<commit_message>
BAB 4 DONE -konka 22apr
</commit_message>
<xml_diff>
--- a/runs/detect/NEW-static_conf/performance-tables.xlsx
+++ b/runs/detect/NEW-static_conf/performance-tables.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redoks\Documents\skripzii\runs\detect\NEW-static_conf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA929D-3865-40C0-976F-C543005F4AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D126157-AC11-496C-B0C1-5236D29FCC2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16044" yWindow="600" windowWidth="7092" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="600" windowWidth="11712" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -479,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>